<commit_message>
Updated compatible tile dimension calculator
</commit_message>
<xml_diff>
--- a/Docs/Other/Compatible_Tile_Calc.xlsx
+++ b/Docs/Other/Compatible_Tile_Calc.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1453924358A\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\JCAP\Docs\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="210" windowWidth="28800" windowHeight="12225"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="18420"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Compatible Tile Dimensions" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -41,14 +41,14 @@
     <t>8x8 V</t>
   </si>
   <si>
-    <t>All zero values represent a compatible dimension for that tile size based on a 640x480 resolution.</t>
+    <t>All green check marks represent a compatible dimension for that tile size based on a 640x480 resolution.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,8 +64,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -90,6 +97,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -319,32 +332,51 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="18">
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -357,17 +389,12 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
           <color indexed="64"/>
         </left>
         <right style="thin">
@@ -379,17 +406,12 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
           <color indexed="64"/>
         </left>
         <right style="medium">
@@ -401,15 +423,12 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
           <color indexed="64"/>
         </left>
         <right style="thin">
@@ -421,17 +440,128 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
           <color indexed="64"/>
         </left>
         <right style="medium">
@@ -441,29 +571,6 @@
           <color indexed="64"/>
         </top>
         <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="medium">
           <color indexed="64"/>
         </bottom>
       </border>
@@ -477,6 +584,23 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -492,23 +616,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="C2:G42" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="C2:G42" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16">
   <autoFilter ref="C2:G42"/>
   <sortState ref="C3:G42">
     <sortCondition ref="C1:C41"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="# Tiles" dataDxfId="2"/>
-    <tableColumn id="2" name="16x16 H" dataDxfId="1">
+    <tableColumn id="1" name="# Tiles" dataDxfId="14"/>
+    <tableColumn id="2" name="16x16 H" dataDxfId="3">
       <calculatedColumnFormula>MOD(640/C3,16)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="16x16 V" dataDxfId="0">
+    <tableColumn id="3" name="16x16 V" dataDxfId="2">
       <calculatedColumnFormula>MOD(480/C3,16)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="8x8 H" dataDxfId="3">
+    <tableColumn id="4" name="8x8 H" dataDxfId="1">
       <calculatedColumnFormula>MOD(640/C3,8)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="8x8 V" dataDxfId="4">
+    <tableColumn id="5" name="8x8 V" dataDxfId="0">
       <calculatedColumnFormula>MOD(480/C3,8)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -781,8 +905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,873 +918,873 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C3" s="16">
+      <c r="C3" s="7">
         <v>1</v>
       </c>
-      <c r="D3" s="7">
-        <f>MOD(640/C3,16)</f>
-        <v>0</v>
-      </c>
-      <c r="E3" s="8">
-        <f>MOD(480/C3,16)</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="13">
-        <f>MOD(640/C3,8)</f>
-        <v>0</v>
-      </c>
-      <c r="G3" s="8">
-        <f>MOD(480/C3,8)</f>
+      <c r="D3" s="10">
+        <f t="shared" ref="D3:D42" si="0">MOD(640/C3,16)</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="11">
+        <f t="shared" ref="E3:E42" si="1">MOD(480/C3,16)</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="12">
+        <f t="shared" ref="F3:F42" si="2">MOD(640/C3,8)</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="11">
+        <f t="shared" ref="G3:G42" si="3">MOD(480/C3,8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C4" s="17">
+      <c r="C4" s="8">
         <v>2</v>
       </c>
-      <c r="D4" s="9">
-        <f>MOD(640/C4,16)</f>
-        <v>0</v>
-      </c>
-      <c r="E4" s="10">
-        <f>MOD(480/C4,16)</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="14">
-        <f>MOD(640/C4,8)</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="10">
-        <f>MOD(480/C4,8)</f>
+      <c r="D4" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E4" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F4" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G4" s="14">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C5" s="17">
+      <c r="C5" s="8">
         <v>3</v>
       </c>
-      <c r="D5" s="9">
-        <f>MOD(640/C5,16)</f>
+      <c r="D5" s="13">
+        <f t="shared" si="0"/>
         <v>5.3333333333333428</v>
       </c>
-      <c r="E5" s="10">
-        <f>MOD(480/C5,16)</f>
-        <v>0</v>
-      </c>
-      <c r="F5" s="14">
-        <f>MOD(640/C5,8)</f>
+      <c r="E5" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F5" s="15">
+        <f t="shared" si="2"/>
         <v>5.3333333333333428</v>
       </c>
-      <c r="G5" s="10">
-        <f>MOD(480/C5,8)</f>
+      <c r="G5" s="14">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C6" s="17">
+      <c r="C6" s="8">
         <v>4</v>
       </c>
-      <c r="D6" s="9">
-        <f>MOD(640/C6,16)</f>
-        <v>0</v>
-      </c>
-      <c r="E6" s="10">
-        <f>MOD(480/C6,16)</f>
+      <c r="D6" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E6" s="14">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="F6" s="14">
-        <f>MOD(640/C6,8)</f>
-        <v>0</v>
-      </c>
-      <c r="G6" s="10">
-        <f>MOD(480/C6,8)</f>
+      <c r="F6" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G6" s="14">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C7" s="17">
+      <c r="C7" s="8">
         <v>5</v>
       </c>
-      <c r="D7" s="9">
-        <f>MOD(640/C7,16)</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="10">
-        <f>MOD(480/C7,16)</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="14">
-        <f>MOD(640/C7,8)</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="10">
-        <f>MOD(480/C7,8)</f>
+      <c r="D7" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E7" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="14">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C8" s="17">
+      <c r="C8" s="8">
         <v>6</v>
       </c>
-      <c r="D8" s="9">
-        <f>MOD(640/C8,16)</f>
+      <c r="D8" s="13">
+        <f t="shared" si="0"/>
         <v>10.666666666666671</v>
       </c>
-      <c r="E8" s="10">
-        <f>MOD(480/C8,16)</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="14">
-        <f>MOD(640/C8,8)</f>
+      <c r="E8" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="15">
+        <f t="shared" si="2"/>
         <v>2.6666666666666714</v>
       </c>
-      <c r="G8" s="10">
-        <f>MOD(480/C8,8)</f>
+      <c r="G8" s="14">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C9" s="17">
+      <c r="C9" s="8">
         <v>7</v>
       </c>
-      <c r="D9" s="9">
-        <f>MOD(640/C9,16)</f>
+      <c r="D9" s="13">
+        <f t="shared" si="0"/>
         <v>11.428571428571431</v>
       </c>
-      <c r="E9" s="10">
-        <f>MOD(480/C9,16)</f>
+      <c r="E9" s="14">
+        <f t="shared" si="1"/>
         <v>4.5714285714285694</v>
       </c>
-      <c r="F9" s="14">
-        <f>MOD(640/C9,8)</f>
+      <c r="F9" s="15">
+        <f t="shared" si="2"/>
         <v>3.4285714285714306</v>
       </c>
-      <c r="G9" s="10">
-        <f>MOD(480/C9,8)</f>
+      <c r="G9" s="14">
+        <f t="shared" si="3"/>
         <v>4.5714285714285694</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C10" s="17">
+      <c r="C10" s="8">
         <v>8</v>
       </c>
-      <c r="D10" s="9">
-        <f>MOD(640/C10,16)</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="10">
-        <f>MOD(480/C10,16)</f>
+      <c r="D10" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E10" s="14">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="F10" s="14">
-        <f>MOD(640/C10,8)</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="10">
-        <f>MOD(480/C10,8)</f>
+      <c r="F10" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="14">
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C11" s="17">
+      <c r="C11" s="8">
         <v>9</v>
       </c>
-      <c r="D11" s="9">
-        <f>MOD(640/C11,16)</f>
+      <c r="D11" s="13">
+        <f t="shared" si="0"/>
         <v>7.1111111111111143</v>
       </c>
-      <c r="E11" s="10">
-        <f>MOD(480/C11,16)</f>
+      <c r="E11" s="14">
+        <f t="shared" si="1"/>
         <v>5.3333333333333357</v>
       </c>
-      <c r="F11" s="14">
-        <f>MOD(640/C11,8)</f>
+      <c r="F11" s="15">
+        <f t="shared" si="2"/>
         <v>7.1111111111111143</v>
       </c>
-      <c r="G11" s="10">
-        <f>MOD(480/C11,8)</f>
+      <c r="G11" s="14">
+        <f t="shared" si="3"/>
         <v>5.3333333333333357</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C12" s="17">
+      <c r="C12" s="8">
         <v>10</v>
       </c>
-      <c r="D12" s="9">
-        <f>MOD(640/C12,16)</f>
-        <v>0</v>
-      </c>
-      <c r="E12" s="10">
-        <f>MOD(480/C12,16)</f>
-        <v>0</v>
-      </c>
-      <c r="F12" s="14">
-        <f>MOD(640/C12,8)</f>
-        <v>0</v>
-      </c>
-      <c r="G12" s="10">
-        <f>MOD(480/C12,8)</f>
+      <c r="D12" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="14">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C13" s="17">
+      <c r="C13" s="8">
         <v>11</v>
       </c>
-      <c r="D13" s="9">
-        <f>MOD(640/C13,16)</f>
+      <c r="D13" s="13">
+        <f t="shared" si="0"/>
         <v>10.18181818181818</v>
       </c>
-      <c r="E13" s="10">
-        <f>MOD(480/C13,16)</f>
+      <c r="E13" s="14">
+        <f t="shared" si="1"/>
         <v>11.636363636363633</v>
       </c>
-      <c r="F13" s="14">
-        <f>MOD(640/C13,8)</f>
+      <c r="F13" s="15">
+        <f t="shared" si="2"/>
         <v>2.1818181818181799</v>
       </c>
-      <c r="G13" s="10">
-        <f>MOD(480/C13,8)</f>
+      <c r="G13" s="14">
+        <f t="shared" si="3"/>
         <v>3.6363636363636331</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C14" s="17">
+      <c r="C14" s="8">
         <v>12</v>
       </c>
-      <c r="D14" s="9">
-        <f>MOD(640/C14,16)</f>
+      <c r="D14" s="13">
+        <f t="shared" si="0"/>
         <v>5.3333333333333357</v>
       </c>
-      <c r="E14" s="10">
-        <f>MOD(480/C14,16)</f>
+      <c r="E14" s="14">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="F14" s="14">
-        <f>MOD(640/C14,8)</f>
+      <c r="F14" s="15">
+        <f t="shared" si="2"/>
         <v>5.3333333333333357</v>
       </c>
-      <c r="G14" s="10">
-        <f>MOD(480/C14,8)</f>
+      <c r="G14" s="14">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C15" s="17">
+      <c r="C15" s="8">
         <v>13</v>
       </c>
-      <c r="D15" s="9">
-        <f>MOD(640/C15,16)</f>
+      <c r="D15" s="13">
+        <f t="shared" si="0"/>
         <v>1.2307692307692335</v>
       </c>
-      <c r="E15" s="10">
-        <f>MOD(480/C15,16)</f>
+      <c r="E15" s="14">
+        <f t="shared" si="1"/>
         <v>4.9230769230769198</v>
       </c>
-      <c r="F15" s="14">
-        <f>MOD(640/C15,8)</f>
+      <c r="F15" s="15">
+        <f t="shared" si="2"/>
         <v>1.2307692307692335</v>
       </c>
-      <c r="G15" s="10">
-        <f>MOD(480/C15,8)</f>
+      <c r="G15" s="14">
+        <f t="shared" si="3"/>
         <v>4.9230769230769198</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C16" s="17">
+      <c r="C16" s="8">
         <v>14</v>
       </c>
-      <c r="D16" s="9">
-        <f>MOD(640/C16,16)</f>
+      <c r="D16" s="13">
+        <f t="shared" si="0"/>
         <v>13.714285714285715</v>
       </c>
-      <c r="E16" s="10">
-        <f>MOD(480/C16,16)</f>
+      <c r="E16" s="14">
+        <f t="shared" si="1"/>
         <v>2.2857142857142847</v>
       </c>
-      <c r="F16" s="14">
-        <f>MOD(640/C16,8)</f>
+      <c r="F16" s="15">
+        <f t="shared" si="2"/>
         <v>5.7142857142857153</v>
       </c>
-      <c r="G16" s="10">
-        <f>MOD(480/C16,8)</f>
+      <c r="G16" s="14">
+        <f t="shared" si="3"/>
         <v>2.2857142857142847</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="17">
+      <c r="C17" s="8">
         <v>15</v>
       </c>
-      <c r="D17" s="9">
-        <f>MOD(640/C17,16)</f>
+      <c r="D17" s="13">
+        <f t="shared" si="0"/>
         <v>10.666666666666664</v>
       </c>
-      <c r="E17" s="10">
-        <f>MOD(480/C17,16)</f>
-        <v>0</v>
-      </c>
-      <c r="F17" s="14">
-        <f>MOD(640/C17,8)</f>
+      <c r="E17" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="15">
+        <f t="shared" si="2"/>
         <v>2.6666666666666643</v>
       </c>
-      <c r="G17" s="10">
-        <f>MOD(480/C17,8)</f>
+      <c r="G17" s="14">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="17">
+      <c r="C18" s="8">
         <v>16</v>
       </c>
-      <c r="D18" s="9">
-        <f>MOD(640/C18,16)</f>
+      <c r="D18" s="13">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E18" s="10">
-        <f>MOD(480/C18,16)</f>
+      <c r="E18" s="14">
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="F18" s="14">
-        <f>MOD(640/C18,8)</f>
-        <v>0</v>
-      </c>
-      <c r="G18" s="10">
-        <f>MOD(480/C18,8)</f>
+      <c r="F18" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="14">
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="17">
+      <c r="C19" s="8">
         <v>17</v>
       </c>
-      <c r="D19" s="9">
-        <f>MOD(640/C19,16)</f>
+      <c r="D19" s="13">
+        <f t="shared" si="0"/>
         <v>5.647058823529413</v>
       </c>
-      <c r="E19" s="10">
-        <f>MOD(480/C19,16)</f>
+      <c r="E19" s="14">
+        <f t="shared" si="1"/>
         <v>12.235294117647058</v>
       </c>
-      <c r="F19" s="14">
-        <f>MOD(640/C19,8)</f>
+      <c r="F19" s="15">
+        <f t="shared" si="2"/>
         <v>5.647058823529413</v>
       </c>
-      <c r="G19" s="10">
-        <f>MOD(480/C19,8)</f>
+      <c r="G19" s="14">
+        <f t="shared" si="3"/>
         <v>4.235294117647058</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="17">
+      <c r="C20" s="8">
         <v>18</v>
       </c>
-      <c r="D20" s="9">
-        <f>MOD(640/C20,16)</f>
+      <c r="D20" s="13">
+        <f t="shared" si="0"/>
         <v>3.5555555555555571</v>
       </c>
-      <c r="E20" s="10">
-        <f>MOD(480/C20,16)</f>
+      <c r="E20" s="14">
+        <f t="shared" si="1"/>
         <v>10.666666666666668</v>
       </c>
-      <c r="F20" s="14">
-        <f>MOD(640/C20,8)</f>
+      <c r="F20" s="15">
+        <f t="shared" si="2"/>
         <v>3.5555555555555571</v>
       </c>
-      <c r="G20" s="10">
-        <f>MOD(480/C20,8)</f>
+      <c r="G20" s="14">
+        <f t="shared" si="3"/>
         <v>2.6666666666666679</v>
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="17">
+      <c r="C21" s="8">
         <v>19</v>
       </c>
-      <c r="D21" s="9">
-        <f>MOD(640/C21,16)</f>
+      <c r="D21" s="13">
+        <f t="shared" si="0"/>
         <v>1.6842105263157876</v>
       </c>
-      <c r="E21" s="10">
-        <f>MOD(480/C21,16)</f>
+      <c r="E21" s="14">
+        <f t="shared" si="1"/>
         <v>9.2631578947368425</v>
       </c>
-      <c r="F21" s="14">
-        <f>MOD(640/C21,8)</f>
+      <c r="F21" s="15">
+        <f t="shared" si="2"/>
         <v>1.6842105263157876</v>
       </c>
-      <c r="G21" s="10">
-        <f>MOD(480/C21,8)</f>
+      <c r="G21" s="14">
+        <f t="shared" si="3"/>
         <v>1.2631578947368425</v>
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="17">
+      <c r="C22" s="8">
         <v>20</v>
       </c>
-      <c r="D22" s="9">
-        <f>MOD(640/C22,16)</f>
-        <v>0</v>
-      </c>
-      <c r="E22" s="10">
-        <f>MOD(480/C22,16)</f>
+      <c r="D22" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E22" s="14">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="F22" s="14">
-        <f>MOD(640/C22,8)</f>
-        <v>0</v>
-      </c>
-      <c r="G22" s="10">
-        <f>MOD(480/C22,8)</f>
+      <c r="F22" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="14">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="17">
+      <c r="C23" s="8">
         <v>21</v>
       </c>
-      <c r="D23" s="9">
-        <f>MOD(640/C23,16)</f>
+      <c r="D23" s="13">
+        <f t="shared" si="0"/>
         <v>14.476190476190474</v>
       </c>
-      <c r="E23" s="10">
-        <f>MOD(480/C23,16)</f>
+      <c r="E23" s="14">
+        <f t="shared" si="1"/>
         <v>6.8571428571428577</v>
       </c>
-      <c r="F23" s="14">
-        <f>MOD(640/C23,8)</f>
+      <c r="F23" s="15">
+        <f t="shared" si="2"/>
         <v>6.4761904761904745</v>
       </c>
-      <c r="G23" s="10">
-        <f>MOD(480/C23,8)</f>
+      <c r="G23" s="14">
+        <f t="shared" si="3"/>
         <v>6.8571428571428577</v>
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="17">
+      <c r="C24" s="8">
         <v>22</v>
       </c>
-      <c r="D24" s="9">
-        <f>MOD(640/C24,16)</f>
+      <c r="D24" s="13">
+        <f t="shared" si="0"/>
         <v>13.09090909090909</v>
       </c>
-      <c r="E24" s="10">
-        <f>MOD(480/C24,16)</f>
+      <c r="E24" s="14">
+        <f t="shared" si="1"/>
         <v>5.8181818181818166</v>
       </c>
-      <c r="F24" s="14">
-        <f>MOD(640/C24,8)</f>
+      <c r="F24" s="15">
+        <f t="shared" si="2"/>
         <v>5.0909090909090899</v>
       </c>
-      <c r="G24" s="10">
-        <f>MOD(480/C24,8)</f>
+      <c r="G24" s="14">
+        <f t="shared" si="3"/>
         <v>5.8181818181818166</v>
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="17">
+      <c r="C25" s="8">
         <v>23</v>
       </c>
-      <c r="D25" s="9">
-        <f>MOD(640/C25,16)</f>
+      <c r="D25" s="13">
+        <f t="shared" si="0"/>
         <v>11.826086956521738</v>
       </c>
-      <c r="E25" s="10">
-        <f>MOD(480/C25,16)</f>
+      <c r="E25" s="14">
+        <f t="shared" si="1"/>
         <v>4.8695652173913047</v>
       </c>
-      <c r="F25" s="14">
-        <f>MOD(640/C25,8)</f>
+      <c r="F25" s="15">
+        <f t="shared" si="2"/>
         <v>3.8260869565217384</v>
       </c>
-      <c r="G25" s="10">
-        <f>MOD(480/C25,8)</f>
+      <c r="G25" s="14">
+        <f t="shared" si="3"/>
         <v>4.8695652173913047</v>
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="17">
+      <c r="C26" s="8">
         <v>24</v>
       </c>
-      <c r="D26" s="9">
-        <f>MOD(640/C26,16)</f>
+      <c r="D26" s="13">
+        <f t="shared" si="0"/>
         <v>10.666666666666668</v>
       </c>
-      <c r="E26" s="10">
-        <f>MOD(480/C26,16)</f>
+      <c r="E26" s="14">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="F26" s="14">
-        <f>MOD(640/C26,8)</f>
+      <c r="F26" s="15">
+        <f t="shared" si="2"/>
         <v>2.6666666666666679</v>
       </c>
-      <c r="G26" s="10">
-        <f>MOD(480/C26,8)</f>
+      <c r="G26" s="14">
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="17">
+      <c r="C27" s="8">
         <v>25</v>
       </c>
-      <c r="D27" s="9">
-        <f>MOD(640/C27,16)</f>
+      <c r="D27" s="13">
+        <f t="shared" si="0"/>
         <v>9.6000000000000014</v>
       </c>
-      <c r="E27" s="10">
-        <f>MOD(480/C27,16)</f>
+      <c r="E27" s="14">
+        <f t="shared" si="1"/>
         <v>3.1999999999999993</v>
       </c>
-      <c r="F27" s="14">
-        <f>MOD(640/C27,8)</f>
+      <c r="F27" s="15">
+        <f t="shared" si="2"/>
         <v>1.6000000000000014</v>
       </c>
-      <c r="G27" s="10">
-        <f>MOD(480/C27,8)</f>
+      <c r="G27" s="14">
+        <f t="shared" si="3"/>
         <v>3.1999999999999993</v>
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="17">
+      <c r="C28" s="8">
         <v>26</v>
       </c>
-      <c r="D28" s="9">
-        <f>MOD(640/C28,16)</f>
+      <c r="D28" s="13">
+        <f t="shared" si="0"/>
         <v>8.6153846153846168</v>
       </c>
-      <c r="E28" s="10">
-        <f>MOD(480/C28,16)</f>
+      <c r="E28" s="14">
+        <f t="shared" si="1"/>
         <v>2.4615384615384599</v>
       </c>
-      <c r="F28" s="14">
-        <f>MOD(640/C28,8)</f>
+      <c r="F28" s="15">
+        <f t="shared" si="2"/>
         <v>0.61538461538461675</v>
       </c>
-      <c r="G28" s="10">
-        <f>MOD(480/C28,8)</f>
+      <c r="G28" s="14">
+        <f t="shared" si="3"/>
         <v>2.4615384615384599</v>
       </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="17">
+      <c r="C29" s="8">
         <v>27</v>
       </c>
-      <c r="D29" s="9">
-        <f>MOD(640/C29,16)</f>
+      <c r="D29" s="13">
+        <f t="shared" si="0"/>
         <v>7.7037037037037024</v>
       </c>
-      <c r="E29" s="10">
-        <f>MOD(480/C29,16)</f>
+      <c r="E29" s="14">
+        <f t="shared" si="1"/>
         <v>1.7777777777777786</v>
       </c>
-      <c r="F29" s="14">
-        <f>MOD(640/C29,8)</f>
+      <c r="F29" s="15">
+        <f t="shared" si="2"/>
         <v>7.7037037037037024</v>
       </c>
-      <c r="G29" s="10">
-        <f>MOD(480/C29,8)</f>
+      <c r="G29" s="14">
+        <f t="shared" si="3"/>
         <v>1.7777777777777786</v>
       </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="17">
+      <c r="C30" s="8">
         <v>28</v>
       </c>
-      <c r="D30" s="9">
-        <f>MOD(640/C30,16)</f>
+      <c r="D30" s="13">
+        <f t="shared" si="0"/>
         <v>6.8571428571428577</v>
       </c>
-      <c r="E30" s="10">
-        <f>MOD(480/C30,16)</f>
+      <c r="E30" s="14">
+        <f t="shared" si="1"/>
         <v>1.1428571428571423</v>
       </c>
-      <c r="F30" s="14">
-        <f>MOD(640/C30,8)</f>
+      <c r="F30" s="15">
+        <f t="shared" si="2"/>
         <v>6.8571428571428577</v>
       </c>
-      <c r="G30" s="10">
-        <f>MOD(480/C30,8)</f>
+      <c r="G30" s="14">
+        <f t="shared" si="3"/>
         <v>1.1428571428571423</v>
       </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C31" s="17">
+      <c r="C31" s="8">
         <v>29</v>
       </c>
-      <c r="D31" s="9">
-        <f>MOD(640/C31,16)</f>
+      <c r="D31" s="13">
+        <f t="shared" si="0"/>
         <v>6.0689655172413808</v>
       </c>
-      <c r="E31" s="10">
-        <f>MOD(480/C31,16)</f>
+      <c r="E31" s="14">
+        <f t="shared" si="1"/>
         <v>0.55172413793103559</v>
       </c>
-      <c r="F31" s="14">
-        <f>MOD(640/C31,8)</f>
+      <c r="F31" s="15">
+        <f t="shared" si="2"/>
         <v>6.0689655172413808</v>
       </c>
-      <c r="G31" s="10">
-        <f>MOD(480/C31,8)</f>
+      <c r="G31" s="14">
+        <f t="shared" si="3"/>
         <v>0.55172413793103559</v>
       </c>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C32" s="17">
+      <c r="C32" s="8">
         <v>30</v>
       </c>
-      <c r="D32" s="9">
-        <f>MOD(640/C32,16)</f>
+      <c r="D32" s="13">
+        <f t="shared" si="0"/>
         <v>5.3333333333333321</v>
       </c>
-      <c r="E32" s="10">
-        <f>MOD(480/C32,16)</f>
-        <v>0</v>
-      </c>
-      <c r="F32" s="14">
-        <f>MOD(640/C32,8)</f>
+      <c r="E32" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="15">
+        <f t="shared" si="2"/>
         <v>5.3333333333333321</v>
       </c>
-      <c r="G32" s="10">
-        <f>MOD(480/C32,8)</f>
+      <c r="G32" s="14">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C33" s="17">
+      <c r="C33" s="8">
         <v>31</v>
       </c>
-      <c r="D33" s="9">
-        <f>MOD(640/C33,16)</f>
+      <c r="D33" s="13">
+        <f t="shared" si="0"/>
         <v>4.6451612903225801</v>
       </c>
-      <c r="E33" s="10">
-        <f>MOD(480/C33,16)</f>
+      <c r="E33" s="14">
+        <f t="shared" si="1"/>
         <v>15.483870967741936</v>
       </c>
-      <c r="F33" s="14">
-        <f>MOD(640/C33,8)</f>
+      <c r="F33" s="15">
+        <f t="shared" si="2"/>
         <v>4.6451612903225801</v>
       </c>
-      <c r="G33" s="10">
-        <f>MOD(480/C33,8)</f>
+      <c r="G33" s="14">
+        <f t="shared" si="3"/>
         <v>7.4838709677419359</v>
       </c>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C34" s="17">
+      <c r="C34" s="8">
         <v>32</v>
       </c>
-      <c r="D34" s="9">
-        <f>MOD(640/C34,16)</f>
+      <c r="D34" s="13">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E34" s="10">
-        <f>MOD(480/C34,16)</f>
+      <c r="E34" s="14">
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="F34" s="14">
-        <f>MOD(640/C34,8)</f>
+      <c r="F34" s="15">
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="G34" s="10">
-        <f>MOD(480/C34,8)</f>
+      <c r="G34" s="14">
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C35" s="17">
+      <c r="C35" s="8">
         <v>33</v>
       </c>
-      <c r="D35" s="9">
-        <f>MOD(640/C35,16)</f>
+      <c r="D35" s="13">
+        <f t="shared" si="0"/>
         <v>3.3939393939393945</v>
       </c>
-      <c r="E35" s="10">
-        <f>MOD(480/C35,16)</f>
+      <c r="E35" s="14">
+        <f t="shared" si="1"/>
         <v>14.545454545454545</v>
       </c>
-      <c r="F35" s="14">
-        <f>MOD(640/C35,8)</f>
+      <c r="F35" s="15">
+        <f t="shared" si="2"/>
         <v>3.3939393939393945</v>
       </c>
-      <c r="G35" s="10">
-        <f>MOD(480/C35,8)</f>
+      <c r="G35" s="14">
+        <f t="shared" si="3"/>
         <v>6.545454545454545</v>
       </c>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C36" s="17">
+      <c r="C36" s="8">
         <v>34</v>
       </c>
-      <c r="D36" s="9">
-        <f>MOD(640/C36,16)</f>
+      <c r="D36" s="13">
+        <f t="shared" si="0"/>
         <v>2.8235294117647065</v>
       </c>
-      <c r="E36" s="10">
-        <f>MOD(480/C36,16)</f>
+      <c r="E36" s="14">
+        <f t="shared" si="1"/>
         <v>14.117647058823529</v>
       </c>
-      <c r="F36" s="14">
-        <f>MOD(640/C36,8)</f>
+      <c r="F36" s="15">
+        <f t="shared" si="2"/>
         <v>2.8235294117647065</v>
       </c>
-      <c r="G36" s="10">
-        <f>MOD(480/C36,8)</f>
+      <c r="G36" s="14">
+        <f t="shared" si="3"/>
         <v>6.117647058823529</v>
       </c>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C37" s="17">
+      <c r="C37" s="8">
         <v>35</v>
       </c>
-      <c r="D37" s="9">
-        <f>MOD(640/C37,16)</f>
+      <c r="D37" s="13">
+        <f t="shared" si="0"/>
         <v>2.2857142857142847</v>
       </c>
-      <c r="E37" s="10">
-        <f>MOD(480/C37,16)</f>
+      <c r="E37" s="14">
+        <f t="shared" si="1"/>
         <v>13.714285714285714</v>
       </c>
-      <c r="F37" s="14">
-        <f>MOD(640/C37,8)</f>
+      <c r="F37" s="15">
+        <f t="shared" si="2"/>
         <v>2.2857142857142847</v>
       </c>
-      <c r="G37" s="10">
-        <f>MOD(480/C37,8)</f>
+      <c r="G37" s="14">
+        <f t="shared" si="3"/>
         <v>5.7142857142857135</v>
       </c>
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C38" s="17">
+      <c r="C38" s="8">
         <v>36</v>
       </c>
-      <c r="D38" s="9">
-        <f>MOD(640/C38,16)</f>
+      <c r="D38" s="13">
+        <f t="shared" si="0"/>
         <v>1.7777777777777786</v>
       </c>
-      <c r="E38" s="10">
-        <f>MOD(480/C38,16)</f>
+      <c r="E38" s="14">
+        <f t="shared" si="1"/>
         <v>13.333333333333334</v>
       </c>
-      <c r="F38" s="14">
-        <f>MOD(640/C38,8)</f>
+      <c r="F38" s="15">
+        <f t="shared" si="2"/>
         <v>1.7777777777777786</v>
       </c>
-      <c r="G38" s="10">
-        <f>MOD(480/C38,8)</f>
+      <c r="G38" s="14">
+        <f t="shared" si="3"/>
         <v>5.3333333333333339</v>
       </c>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C39" s="17">
+      <c r="C39" s="8">
         <v>37</v>
       </c>
-      <c r="D39" s="9">
-        <f>MOD(640/C39,16)</f>
+      <c r="D39" s="13">
+        <f t="shared" si="0"/>
         <v>1.2972972972972983</v>
       </c>
-      <c r="E39" s="10">
-        <f>MOD(480/C39,16)</f>
+      <c r="E39" s="14">
+        <f t="shared" si="1"/>
         <v>12.972972972972974</v>
       </c>
-      <c r="F39" s="14">
-        <f>MOD(640/C39,8)</f>
+      <c r="F39" s="15">
+        <f t="shared" si="2"/>
         <v>1.2972972972972983</v>
       </c>
-      <c r="G39" s="10">
-        <f>MOD(480/C39,8)</f>
+      <c r="G39" s="14">
+        <f t="shared" si="3"/>
         <v>4.9729729729729737</v>
       </c>
     </row>
     <row r="40" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C40" s="17">
+      <c r="C40" s="8">
         <v>38</v>
       </c>
-      <c r="D40" s="9">
-        <f>MOD(640/C40,16)</f>
+      <c r="D40" s="13">
+        <f t="shared" si="0"/>
         <v>0.8421052631578938</v>
       </c>
-      <c r="E40" s="10">
-        <f>MOD(480/C40,16)</f>
+      <c r="E40" s="14">
+        <f t="shared" si="1"/>
         <v>12.631578947368421</v>
       </c>
-      <c r="F40" s="14">
-        <f>MOD(640/C40,8)</f>
+      <c r="F40" s="15">
+        <f t="shared" si="2"/>
         <v>0.8421052631578938</v>
       </c>
-      <c r="G40" s="10">
-        <f>MOD(480/C40,8)</f>
+      <c r="G40" s="14">
+        <f t="shared" si="3"/>
         <v>4.6315789473684212</v>
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C41" s="17">
+      <c r="C41" s="8">
         <v>39</v>
       </c>
-      <c r="D41" s="9">
-        <f>MOD(640/C41,16)</f>
+      <c r="D41" s="13">
+        <f t="shared" si="0"/>
         <v>0.4102564102564088</v>
       </c>
-      <c r="E41" s="10">
-        <f>MOD(480/C41,16)</f>
+      <c r="E41" s="14">
+        <f t="shared" si="1"/>
         <v>12.307692307692308</v>
       </c>
-      <c r="F41" s="14">
-        <f>MOD(640/C41,8)</f>
+      <c r="F41" s="15">
+        <f t="shared" si="2"/>
         <v>0.4102564102564088</v>
       </c>
-      <c r="G41" s="10">
-        <f>MOD(480/C41,8)</f>
+      <c r="G41" s="14">
+        <f t="shared" si="3"/>
         <v>4.3076923076923084</v>
       </c>
     </row>
     <row r="42" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C42" s="18">
+      <c r="C42" s="9">
         <v>40</v>
       </c>
-      <c r="D42" s="11">
-        <f>MOD(640/C42,16)</f>
-        <v>0</v>
-      </c>
-      <c r="E42" s="12">
-        <f>MOD(480/C42,16)</f>
+      <c r="D42" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E42" s="17">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="F42" s="15">
-        <f>MOD(640/C42,8)</f>
-        <v>0</v>
-      </c>
-      <c r="G42" s="12">
-        <f>MOD(480/C42,8)</f>
+      <c r="F42" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G42" s="17">
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
     </row>
@@ -1669,7 +1793,10 @@
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:G42">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="3" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1678,5 +1805,30 @@
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="1" id="{12E85491-EDF6-4C2C-AC8B-C08E42EDF740}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>D3:G42</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated tile dimension calc
</commit_message>
<xml_diff>
--- a/Docs/Other/Compatible_Tile_Calc.xlsx
+++ b/Docs/Other/Compatible_Tile_Calc.xlsx
@@ -336,9 +336,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -369,79 +366,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -463,84 +395,72 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -574,16 +494,6 @@
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <border>
@@ -616,23 +526,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="C2:G42" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="C2:G42" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7">
   <autoFilter ref="C2:G42"/>
   <sortState ref="C3:G42">
     <sortCondition ref="C1:C41"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="# Tiles" dataDxfId="14"/>
-    <tableColumn id="2" name="16x16 H" dataDxfId="3">
+    <tableColumn id="1" name="# Tiles" dataDxfId="6"/>
+    <tableColumn id="2" name="16x16 H" dataDxfId="5">
       <calculatedColumnFormula>MOD(640/C3,16)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="16x16 V" dataDxfId="2">
+    <tableColumn id="3" name="16x16 V" dataDxfId="4">
       <calculatedColumnFormula>MOD(480/C3,16)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="8x8 H" dataDxfId="1">
+    <tableColumn id="4" name="8x8 H" dataDxfId="3">
       <calculatedColumnFormula>MOD(640/C3,8)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="8x8 V" dataDxfId="0">
+    <tableColumn id="5" name="8x8 V" dataDxfId="2">
       <calculatedColumnFormula>MOD(480/C3,8)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -906,7 +816,7 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,17 +828,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -949,841 +859,841 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>1</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="9">
         <f t="shared" ref="D3:D42" si="0">MOD(640/C3,16)</f>
         <v>0</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="10">
         <f t="shared" ref="E3:E42" si="1">MOD(480/C3,16)</f>
         <v>0</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="11">
         <f t="shared" ref="F3:F42" si="2">MOD(640/C3,8)</f>
         <v>0</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="10">
         <f t="shared" ref="G3:G42" si="3">MOD(480/C3,8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>2</v>
       </c>
-      <c r="D4" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E4" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F4" s="15">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G4" s="14">
+      <c r="D4" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E4" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F4" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G4" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>3</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="12">
         <f t="shared" si="0"/>
         <v>5.3333333333333428</v>
       </c>
-      <c r="E5" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F5" s="15">
+      <c r="E5" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F5" s="14">
         <f t="shared" si="2"/>
         <v>5.3333333333333428</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <v>4</v>
       </c>
-      <c r="D6" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E6" s="14">
+      <c r="D6" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E6" s="13">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="F6" s="15">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G6" s="14">
+      <c r="F6" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G6" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>5</v>
       </c>
-      <c r="D7" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E7" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F7" s="15">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G7" s="14">
+      <c r="D7" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E7" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C8" s="8">
+      <c r="C8" s="7">
         <v>6</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="12">
         <f t="shared" si="0"/>
         <v>10.666666666666671</v>
       </c>
-      <c r="E8" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F8" s="15">
+      <c r="E8" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="14">
         <f t="shared" si="2"/>
         <v>2.6666666666666714</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C9" s="8">
+      <c r="C9" s="7">
         <v>7</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="12">
         <f t="shared" si="0"/>
         <v>11.428571428571431</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="13">
         <f t="shared" si="1"/>
         <v>4.5714285714285694</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="14">
         <f t="shared" si="2"/>
         <v>3.4285714285714306</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="13">
         <f t="shared" si="3"/>
         <v>4.5714285714285694</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C10" s="8">
+      <c r="C10" s="7">
         <v>8</v>
       </c>
-      <c r="D10" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E10" s="14">
+      <c r="D10" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E10" s="13">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="F10" s="15">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G10" s="14">
+      <c r="F10" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="13">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C11" s="8">
+      <c r="C11" s="7">
         <v>9</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="12">
         <f t="shared" si="0"/>
         <v>7.1111111111111143</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="13">
         <f t="shared" si="1"/>
         <v>5.3333333333333357</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="14">
         <f t="shared" si="2"/>
         <v>7.1111111111111143</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="13">
         <f t="shared" si="3"/>
         <v>5.3333333333333357</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>10</v>
       </c>
-      <c r="D12" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E12" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="15">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="14">
+      <c r="D12" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C13" s="8">
+      <c r="C13" s="7">
         <v>11</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="12">
         <f t="shared" si="0"/>
         <v>10.18181818181818</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="13">
         <f t="shared" si="1"/>
         <v>11.636363636363633</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="14">
         <f t="shared" si="2"/>
         <v>2.1818181818181799</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="13">
         <f t="shared" si="3"/>
         <v>3.6363636363636331</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C14" s="8">
+      <c r="C14" s="7">
         <v>12</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="12">
         <f t="shared" si="0"/>
         <v>5.3333333333333357</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="13">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="14">
         <f t="shared" si="2"/>
         <v>5.3333333333333357</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G14" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C15" s="8">
+      <c r="C15" s="7">
         <v>13</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="12">
         <f t="shared" si="0"/>
         <v>1.2307692307692335</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="13">
         <f t="shared" si="1"/>
         <v>4.9230769230769198</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="14">
         <f t="shared" si="2"/>
         <v>1.2307692307692335</v>
       </c>
-      <c r="G15" s="14">
+      <c r="G15" s="13">
         <f t="shared" si="3"/>
         <v>4.9230769230769198</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C16" s="8">
+      <c r="C16" s="7">
         <v>14</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="12">
         <f t="shared" si="0"/>
         <v>13.714285714285715</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="13">
         <f t="shared" si="1"/>
         <v>2.2857142857142847</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="14">
         <f t="shared" si="2"/>
         <v>5.7142857142857153</v>
       </c>
-      <c r="G16" s="14">
+      <c r="G16" s="13">
         <f t="shared" si="3"/>
         <v>2.2857142857142847</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="8">
+      <c r="C17" s="7">
         <v>15</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="12">
         <f t="shared" si="0"/>
         <v>10.666666666666664</v>
       </c>
-      <c r="E17" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="15">
+      <c r="E17" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="14">
         <f t="shared" si="2"/>
         <v>2.6666666666666643</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="8">
+      <c r="C18" s="7">
         <v>16</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="12">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="13">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="F18" s="15">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="14">
+      <c r="F18" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="13">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="8">
+      <c r="C19" s="7">
         <v>17</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D19" s="12">
         <f t="shared" si="0"/>
         <v>5.647058823529413</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="13">
         <f t="shared" si="1"/>
         <v>12.235294117647058</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F19" s="14">
         <f t="shared" si="2"/>
         <v>5.647058823529413</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G19" s="13">
         <f t="shared" si="3"/>
         <v>4.235294117647058</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="8">
+      <c r="C20" s="7">
         <v>18</v>
       </c>
-      <c r="D20" s="13">
+      <c r="D20" s="12">
         <f t="shared" si="0"/>
         <v>3.5555555555555571</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="13">
         <f t="shared" si="1"/>
         <v>10.666666666666668</v>
       </c>
-      <c r="F20" s="15">
+      <c r="F20" s="14">
         <f t="shared" si="2"/>
         <v>3.5555555555555571</v>
       </c>
-      <c r="G20" s="14">
+      <c r="G20" s="13">
         <f t="shared" si="3"/>
         <v>2.6666666666666679</v>
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="8">
+      <c r="C21" s="7">
         <v>19</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D21" s="12">
         <f t="shared" si="0"/>
         <v>1.6842105263157876</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21" s="13">
         <f t="shared" si="1"/>
         <v>9.2631578947368425</v>
       </c>
-      <c r="F21" s="15">
+      <c r="F21" s="14">
         <f t="shared" si="2"/>
         <v>1.6842105263157876</v>
       </c>
-      <c r="G21" s="14">
+      <c r="G21" s="13">
         <f t="shared" si="3"/>
         <v>1.2631578947368425</v>
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="8">
+      <c r="C22" s="7">
         <v>20</v>
       </c>
-      <c r="D22" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E22" s="14">
+      <c r="D22" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E22" s="13">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="F22" s="15">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G22" s="14">
+      <c r="F22" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="8">
+      <c r="C23" s="7">
         <v>21</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D23" s="12">
         <f t="shared" si="0"/>
         <v>14.476190476190474</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E23" s="13">
         <f t="shared" si="1"/>
         <v>6.8571428571428577</v>
       </c>
-      <c r="F23" s="15">
+      <c r="F23" s="14">
         <f t="shared" si="2"/>
         <v>6.4761904761904745</v>
       </c>
-      <c r="G23" s="14">
+      <c r="G23" s="13">
         <f t="shared" si="3"/>
         <v>6.8571428571428577</v>
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="8">
+      <c r="C24" s="7">
         <v>22</v>
       </c>
-      <c r="D24" s="13">
+      <c r="D24" s="12">
         <f t="shared" si="0"/>
         <v>13.09090909090909</v>
       </c>
-      <c r="E24" s="14">
+      <c r="E24" s="13">
         <f t="shared" si="1"/>
         <v>5.8181818181818166</v>
       </c>
-      <c r="F24" s="15">
+      <c r="F24" s="14">
         <f t="shared" si="2"/>
         <v>5.0909090909090899</v>
       </c>
-      <c r="G24" s="14">
+      <c r="G24" s="13">
         <f t="shared" si="3"/>
         <v>5.8181818181818166</v>
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="8">
+      <c r="C25" s="7">
         <v>23</v>
       </c>
-      <c r="D25" s="13">
+      <c r="D25" s="12">
         <f t="shared" si="0"/>
         <v>11.826086956521738</v>
       </c>
-      <c r="E25" s="14">
+      <c r="E25" s="13">
         <f t="shared" si="1"/>
         <v>4.8695652173913047</v>
       </c>
-      <c r="F25" s="15">
+      <c r="F25" s="14">
         <f t="shared" si="2"/>
         <v>3.8260869565217384</v>
       </c>
-      <c r="G25" s="14">
+      <c r="G25" s="13">
         <f t="shared" si="3"/>
         <v>4.8695652173913047</v>
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="8">
+      <c r="C26" s="7">
         <v>24</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D26" s="12">
         <f t="shared" si="0"/>
         <v>10.666666666666668</v>
       </c>
-      <c r="E26" s="14">
+      <c r="E26" s="13">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="F26" s="15">
+      <c r="F26" s="14">
         <f t="shared" si="2"/>
         <v>2.6666666666666679</v>
       </c>
-      <c r="G26" s="14">
+      <c r="G26" s="13">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="8">
+      <c r="C27" s="7">
         <v>25</v>
       </c>
-      <c r="D27" s="13">
+      <c r="D27" s="12">
         <f t="shared" si="0"/>
         <v>9.6000000000000014</v>
       </c>
-      <c r="E27" s="14">
+      <c r="E27" s="13">
         <f t="shared" si="1"/>
         <v>3.1999999999999993</v>
       </c>
-      <c r="F27" s="15">
+      <c r="F27" s="14">
         <f t="shared" si="2"/>
         <v>1.6000000000000014</v>
       </c>
-      <c r="G27" s="14">
+      <c r="G27" s="13">
         <f t="shared" si="3"/>
         <v>3.1999999999999993</v>
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="8">
+      <c r="C28" s="7">
         <v>26</v>
       </c>
-      <c r="D28" s="13">
+      <c r="D28" s="12">
         <f t="shared" si="0"/>
         <v>8.6153846153846168</v>
       </c>
-      <c r="E28" s="14">
+      <c r="E28" s="13">
         <f t="shared" si="1"/>
         <v>2.4615384615384599</v>
       </c>
-      <c r="F28" s="15">
+      <c r="F28" s="14">
         <f t="shared" si="2"/>
         <v>0.61538461538461675</v>
       </c>
-      <c r="G28" s="14">
+      <c r="G28" s="13">
         <f t="shared" si="3"/>
         <v>2.4615384615384599</v>
       </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="8">
+      <c r="C29" s="7">
         <v>27</v>
       </c>
-      <c r="D29" s="13">
+      <c r="D29" s="12">
         <f t="shared" si="0"/>
         <v>7.7037037037037024</v>
       </c>
-      <c r="E29" s="14">
+      <c r="E29" s="13">
         <f t="shared" si="1"/>
         <v>1.7777777777777786</v>
       </c>
-      <c r="F29" s="15">
+      <c r="F29" s="14">
         <f t="shared" si="2"/>
         <v>7.7037037037037024</v>
       </c>
-      <c r="G29" s="14">
+      <c r="G29" s="13">
         <f t="shared" si="3"/>
         <v>1.7777777777777786</v>
       </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="8">
+      <c r="C30" s="7">
         <v>28</v>
       </c>
-      <c r="D30" s="13">
+      <c r="D30" s="12">
         <f t="shared" si="0"/>
         <v>6.8571428571428577</v>
       </c>
-      <c r="E30" s="14">
+      <c r="E30" s="13">
         <f t="shared" si="1"/>
         <v>1.1428571428571423</v>
       </c>
-      <c r="F30" s="15">
+      <c r="F30" s="14">
         <f t="shared" si="2"/>
         <v>6.8571428571428577</v>
       </c>
-      <c r="G30" s="14">
+      <c r="G30" s="13">
         <f t="shared" si="3"/>
         <v>1.1428571428571423</v>
       </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C31" s="8">
+      <c r="C31" s="7">
         <v>29</v>
       </c>
-      <c r="D31" s="13">
+      <c r="D31" s="12">
         <f t="shared" si="0"/>
         <v>6.0689655172413808</v>
       </c>
-      <c r="E31" s="14">
+      <c r="E31" s="13">
         <f t="shared" si="1"/>
         <v>0.55172413793103559</v>
       </c>
-      <c r="F31" s="15">
+      <c r="F31" s="14">
         <f t="shared" si="2"/>
         <v>6.0689655172413808</v>
       </c>
-      <c r="G31" s="14">
+      <c r="G31" s="13">
         <f t="shared" si="3"/>
         <v>0.55172413793103559</v>
       </c>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C32" s="8">
+      <c r="C32" s="7">
         <v>30</v>
       </c>
-      <c r="D32" s="13">
+      <c r="D32" s="12">
         <f t="shared" si="0"/>
         <v>5.3333333333333321</v>
       </c>
-      <c r="E32" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F32" s="15">
+      <c r="E32" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="14">
         <f t="shared" si="2"/>
         <v>5.3333333333333321</v>
       </c>
-      <c r="G32" s="14">
+      <c r="G32" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C33" s="8">
+      <c r="C33" s="7">
         <v>31</v>
       </c>
-      <c r="D33" s="13">
+      <c r="D33" s="12">
         <f t="shared" si="0"/>
         <v>4.6451612903225801</v>
       </c>
-      <c r="E33" s="14">
+      <c r="E33" s="13">
         <f t="shared" si="1"/>
         <v>15.483870967741936</v>
       </c>
-      <c r="F33" s="15">
+      <c r="F33" s="14">
         <f t="shared" si="2"/>
         <v>4.6451612903225801</v>
       </c>
-      <c r="G33" s="14">
+      <c r="G33" s="13">
         <f t="shared" si="3"/>
         <v>7.4838709677419359</v>
       </c>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C34" s="8">
+      <c r="C34" s="7">
         <v>32</v>
       </c>
-      <c r="D34" s="13">
+      <c r="D34" s="12">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E34" s="14">
+      <c r="E34" s="13">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="F34" s="15">
+      <c r="F34" s="14">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="G34" s="14">
+      <c r="G34" s="13">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C35" s="8">
+      <c r="C35" s="7">
         <v>33</v>
       </c>
-      <c r="D35" s="13">
+      <c r="D35" s="12">
         <f t="shared" si="0"/>
         <v>3.3939393939393945</v>
       </c>
-      <c r="E35" s="14">
+      <c r="E35" s="13">
         <f t="shared" si="1"/>
         <v>14.545454545454545</v>
       </c>
-      <c r="F35" s="15">
+      <c r="F35" s="14">
         <f t="shared" si="2"/>
         <v>3.3939393939393945</v>
       </c>
-      <c r="G35" s="14">
+      <c r="G35" s="13">
         <f t="shared" si="3"/>
         <v>6.545454545454545</v>
       </c>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C36" s="8">
+      <c r="C36" s="7">
         <v>34</v>
       </c>
-      <c r="D36" s="13">
+      <c r="D36" s="12">
         <f t="shared" si="0"/>
         <v>2.8235294117647065</v>
       </c>
-      <c r="E36" s="14">
+      <c r="E36" s="13">
         <f t="shared" si="1"/>
         <v>14.117647058823529</v>
       </c>
-      <c r="F36" s="15">
+      <c r="F36" s="14">
         <f t="shared" si="2"/>
         <v>2.8235294117647065</v>
       </c>
-      <c r="G36" s="14">
+      <c r="G36" s="13">
         <f t="shared" si="3"/>
         <v>6.117647058823529</v>
       </c>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C37" s="8">
+      <c r="C37" s="7">
         <v>35</v>
       </c>
-      <c r="D37" s="13">
+      <c r="D37" s="12">
         <f t="shared" si="0"/>
         <v>2.2857142857142847</v>
       </c>
-      <c r="E37" s="14">
+      <c r="E37" s="13">
         <f t="shared" si="1"/>
         <v>13.714285714285714</v>
       </c>
-      <c r="F37" s="15">
+      <c r="F37" s="14">
         <f t="shared" si="2"/>
         <v>2.2857142857142847</v>
       </c>
-      <c r="G37" s="14">
+      <c r="G37" s="13">
         <f t="shared" si="3"/>
         <v>5.7142857142857135</v>
       </c>
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C38" s="8">
+      <c r="C38" s="7">
         <v>36</v>
       </c>
-      <c r="D38" s="13">
+      <c r="D38" s="12">
         <f t="shared" si="0"/>
         <v>1.7777777777777786</v>
       </c>
-      <c r="E38" s="14">
+      <c r="E38" s="13">
         <f t="shared" si="1"/>
         <v>13.333333333333334</v>
       </c>
-      <c r="F38" s="15">
+      <c r="F38" s="14">
         <f t="shared" si="2"/>
         <v>1.7777777777777786</v>
       </c>
-      <c r="G38" s="14">
+      <c r="G38" s="13">
         <f t="shared" si="3"/>
         <v>5.3333333333333339</v>
       </c>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C39" s="8">
+      <c r="C39" s="7">
         <v>37</v>
       </c>
-      <c r="D39" s="13">
+      <c r="D39" s="12">
         <f t="shared" si="0"/>
         <v>1.2972972972972983</v>
       </c>
-      <c r="E39" s="14">
+      <c r="E39" s="13">
         <f t="shared" si="1"/>
         <v>12.972972972972974</v>
       </c>
-      <c r="F39" s="15">
+      <c r="F39" s="14">
         <f t="shared" si="2"/>
         <v>1.2972972972972983</v>
       </c>
-      <c r="G39" s="14">
+      <c r="G39" s="13">
         <f t="shared" si="3"/>
         <v>4.9729729729729737</v>
       </c>
     </row>
     <row r="40" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C40" s="8">
+      <c r="C40" s="7">
         <v>38</v>
       </c>
-      <c r="D40" s="13">
+      <c r="D40" s="12">
         <f t="shared" si="0"/>
         <v>0.8421052631578938</v>
       </c>
-      <c r="E40" s="14">
+      <c r="E40" s="13">
         <f t="shared" si="1"/>
         <v>12.631578947368421</v>
       </c>
-      <c r="F40" s="15">
+      <c r="F40" s="14">
         <f t="shared" si="2"/>
         <v>0.8421052631578938</v>
       </c>
-      <c r="G40" s="14">
+      <c r="G40" s="13">
         <f t="shared" si="3"/>
         <v>4.6315789473684212</v>
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C41" s="8">
+      <c r="C41" s="7">
         <v>39</v>
       </c>
-      <c r="D41" s="13">
+      <c r="D41" s="12">
         <f t="shared" si="0"/>
         <v>0.4102564102564088</v>
       </c>
-      <c r="E41" s="14">
+      <c r="E41" s="13">
         <f t="shared" si="1"/>
         <v>12.307692307692308</v>
       </c>
-      <c r="F41" s="15">
+      <c r="F41" s="14">
         <f t="shared" si="2"/>
         <v>0.4102564102564088</v>
       </c>
-      <c r="G41" s="14">
+      <c r="G41" s="13">
         <f t="shared" si="3"/>
         <v>4.3076923076923084</v>
       </c>
     </row>
     <row r="42" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C42" s="9">
+      <c r="C42" s="8">
         <v>40</v>
       </c>
-      <c r="D42" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E42" s="17">
+      <c r="D42" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E42" s="16">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="F42" s="18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G42" s="17">
+      <c r="F42" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G42" s="16">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
@@ -1793,10 +1703,10 @@
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:G42">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1821,7 +1731,7 @@
                 <xm:f>1</xm:f>
               </x14:cfvo>
               <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
               <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>

</xml_diff>